<commit_message>
Fixed Game of life excel example Fixed Board strategies Fixed Cell constructor and game of life function Minor fixes to Layer Added looping to View Minor fixes to File reader
</commit_message>
<xml_diff>
--- a/Examples/Game of Life/excel/example.xlsx
+++ b/Examples/Game of Life/excel/example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wikto\PycharmProjects\MasterDegree\Examples\Game of Life\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wikto\Desktop\homework\MasterDegree\Examples\Game of Life\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803CDC63-0A33-45B3-B3B5-B81D88BF01D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B29AAE-B669-4CFC-BC4B-0E6CE5172FE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2205" windowWidth="21600" windowHeight="11835" xr2:uid="{CACAD4C5-5037-44B5-AF02-A22C5524F177}"/>
+    <workbookView xWindow="-23148" yWindow="4188" windowWidth="23256" windowHeight="13176" xr2:uid="{CACAD4C5-5037-44B5-AF02-A22C5524F177}"/>
   </bookViews>
   <sheets>
     <sheet name="Layer" sheetId="1" r:id="rId1"/>
@@ -396,25 +396,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A73E6186-CDDF-496E-A379-AE8DB6C0E685}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -463,8 +463,14 @@
       <c r="P4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -513,8 +519,14 @@
       <c r="P5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -563,8 +575,14 @@
       <c r="P6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -613,8 +631,14 @@
       <c r="P7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -663,8 +687,14 @@
       <c r="P8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -674,13 +704,13 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9">
@@ -698,13 +728,13 @@
       <c r="K9">
         <v>0</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <v>0</v>
       </c>
       <c r="O9">
@@ -713,27 +743,33 @@
       <c r="P9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
         <v>0</v>
       </c>
       <c r="H10">
@@ -745,45 +781,51 @@
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
-      <c r="L10">
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
         <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-      <c r="O10">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
         <v>0</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
         <v>0</v>
       </c>
       <c r="H11">
@@ -795,45 +837,51 @@
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
         <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-      <c r="O11">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
         <v>0</v>
       </c>
       <c r="P11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12">
@@ -845,26 +893,32 @@
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
         <v>0</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -874,13 +928,13 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>0</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>0</v>
       </c>
       <c r="G13">
@@ -898,13 +952,13 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" s="1">
         <v>0</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="1">
         <v>0</v>
       </c>
       <c r="O13">
@@ -913,8 +967,14 @@
       <c r="P13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -963,8 +1023,14 @@
       <c r="P14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1013,8 +1079,14 @@
       <c r="P15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -1063,8 +1135,14 @@
       <c r="P16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -1113,8 +1191,14 @@
       <c r="P17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -1163,8 +1247,14 @@
       <c r="P18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -1213,9 +1303,127 @@
       <c r="P19">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>